<commit_message>
Added a comment fo fix confusion
</commit_message>
<xml_diff>
--- a/circadian rev2.1/circad 2.1 bom.xlsx
+++ b/circadian rev2.1/circad 2.1 bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marec\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB417A94-867D-43A5-9044-E8BB0153255C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D53041-956D-4CD9-B03D-EE6E19C58D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,9 +332,6 @@
     <t xml:space="preserve">688-EC11E18244A5 </t>
   </si>
   <si>
-    <t>SK6812 3535</t>
-  </si>
-  <si>
     <t>SK6812 3535 RGB LED</t>
   </si>
   <si>
@@ -354,6 +351,9 @@
   </si>
   <si>
     <t>R13 - R16, R23</t>
+  </si>
+  <si>
+    <t>SK6812 3535 (chip inside must be facing side with no leads - up on the PCB)</t>
   </si>
 </sst>
 </file>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
@@ -994,7 +994,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="27.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1061,22 +1061,22 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="13">
         <v>72</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>99</v>
+      <c r="C4" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="13">
         <v>3535</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1239,7 +1239,7 @@
     </row>
     <row r="10" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="13">
         <v>5</v>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="14" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" s="13">
         <v>2</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="20" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" s="13">
         <v>1</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="21" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="13">
         <v>1</v>
@@ -1880,7 +1880,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>23</v>

</xml_diff>